<commit_message>
Fix file Excel for HR
</commit_message>
<xml_diff>
--- a/WindowsFormsApplication1/Resources/AttendanceDaily.xlsx
+++ b/WindowsFormsApplication1/Resources/AttendanceDaily.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\DevelopeHRSoftware\WindowsFormsApplication1\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\Techlink_Software_Development\WindowsFormsApplication1\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1058,10 +1058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S113"/>
+  <dimension ref="A1:S116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I108" sqref="I108"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3358,7 +3358,7 @@
       <c r="H76" s="13"/>
       <c r="I76" s="13"/>
       <c r="J76" s="14">
-        <f t="shared" ref="J76:J108" si="6">K76+P76+Q76</f>
+        <f t="shared" ref="J76:J111" si="6">K76+P76+Q76</f>
         <v>0</v>
       </c>
       <c r="K76" s="21"/>
@@ -3898,18 +3898,18 @@
       <c r="H94" s="19"/>
       <c r="I94" s="19"/>
       <c r="J94" s="14">
-        <f t="shared" ref="J94:J99" si="7">K94+P94+Q94</f>
+        <f t="shared" ref="J94:J110" si="7">K94+P94+Q94</f>
         <v>0</v>
       </c>
       <c r="K94" s="21"/>
       <c r="L94" s="21"/>
       <c r="M94" s="21"/>
       <c r="N94" s="14">
-        <f t="shared" ref="N94:N99" si="8">G94+I94</f>
+        <f t="shared" ref="N94:O110" si="8">G94+I94</f>
         <v>0</v>
       </c>
       <c r="O94" s="14">
-        <f t="shared" ref="O94:O99" si="9">F94+H94</f>
+        <f t="shared" ref="O94:O110" si="9">F94+H94</f>
         <v>0</v>
       </c>
       <c r="P94" s="16"/>
@@ -3969,7 +3969,7 @@
         <v>0</v>
       </c>
       <c r="O96" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P96" s="16"/>
@@ -3999,7 +3999,7 @@
         <v>0</v>
       </c>
       <c r="O97" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P97" s="16"/>
@@ -4029,7 +4029,7 @@
         <v>0</v>
       </c>
       <c r="O98" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P98" s="16"/>
@@ -4059,7 +4059,7 @@
         <v>0</v>
       </c>
       <c r="O99" s="14">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P99" s="16"/>
@@ -4078,18 +4078,18 @@
       <c r="H100" s="19"/>
       <c r="I100" s="19"/>
       <c r="J100" s="14">
-        <f t="shared" ref="J100:J101" si="10">K100+P100+Q100</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K100" s="14"/>
       <c r="L100" s="16"/>
       <c r="M100" s="16"/>
       <c r="N100" s="14">
-        <f t="shared" ref="N100:N101" si="11">G100+I100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O100" s="14">
-        <f t="shared" ref="O100:O101" si="12">F100+H100</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P100" s="16"/>
@@ -4101,25 +4101,25 @@
       <c r="A101" s="28"/>
       <c r="B101" s="16"/>
       <c r="C101" s="16"/>
-      <c r="D101" s="17"/>
-      <c r="E101" s="17"/>
+      <c r="D101" s="26"/>
+      <c r="E101" s="27"/>
       <c r="F101" s="14"/>
-      <c r="G101" s="19"/>
+      <c r="G101" s="16"/>
       <c r="H101" s="19"/>
       <c r="I101" s="19"/>
       <c r="J101" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K101" s="14"/>
       <c r="L101" s="16"/>
       <c r="M101" s="16"/>
       <c r="N101" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="O101" s="14">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="P101" s="16"/>
@@ -4131,10 +4131,10 @@
       <c r="A102" s="28"/>
       <c r="B102" s="16"/>
       <c r="C102" s="16"/>
-      <c r="D102" s="17"/>
-      <c r="E102" s="17"/>
+      <c r="D102" s="26"/>
+      <c r="E102" s="27"/>
       <c r="F102" s="14"/>
-      <c r="G102" s="19"/>
+      <c r="G102" s="16"/>
       <c r="H102" s="19"/>
       <c r="I102" s="19"/>
       <c r="J102" s="14">
@@ -4158,10 +4158,10 @@
       <c r="A103" s="28"/>
       <c r="B103" s="16"/>
       <c r="C103" s="16"/>
-      <c r="D103" s="17"/>
-      <c r="E103" s="17"/>
+      <c r="D103" s="26"/>
+      <c r="E103" s="27"/>
       <c r="F103" s="14"/>
-      <c r="G103" s="19"/>
+      <c r="G103" s="16"/>
       <c r="H103" s="19"/>
       <c r="I103" s="19"/>
       <c r="J103" s="14">
@@ -4185,10 +4185,10 @@
       <c r="A104" s="28"/>
       <c r="B104" s="16"/>
       <c r="C104" s="16"/>
-      <c r="D104" s="17"/>
-      <c r="E104" s="17"/>
+      <c r="D104" s="26"/>
+      <c r="E104" s="27"/>
       <c r="F104" s="14"/>
-      <c r="G104" s="19"/>
+      <c r="G104" s="16"/>
       <c r="H104" s="19"/>
       <c r="I104" s="19"/>
       <c r="J104" s="14">
@@ -4212,25 +4212,25 @@
       <c r="A105" s="28"/>
       <c r="B105" s="16"/>
       <c r="C105" s="16"/>
-      <c r="D105" s="15"/>
-      <c r="E105" s="15"/>
+      <c r="D105" s="26"/>
+      <c r="E105" s="27"/>
       <c r="F105" s="14"/>
-      <c r="G105" s="19"/>
+      <c r="G105" s="16"/>
       <c r="H105" s="19"/>
       <c r="I105" s="19"/>
       <c r="J105" s="14">
-        <f t="shared" ref="J105" si="13">K105+P105+Q105</f>
+        <f t="shared" ref="J105" si="10">K105+P105+Q105</f>
         <v>0</v>
       </c>
       <c r="K105" s="14"/>
       <c r="L105" s="16"/>
       <c r="M105" s="16"/>
       <c r="N105" s="14">
-        <f t="shared" ref="N105" si="14">G105+I105</f>
+        <f t="shared" ref="N105:O105" si="11">G105+I105</f>
         <v>0</v>
       </c>
       <c r="O105" s="14">
-        <f t="shared" ref="O105" si="15">F105+H105</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P105" s="16"/>
@@ -4242,10 +4242,10 @@
       <c r="A106" s="28"/>
       <c r="B106" s="16"/>
       <c r="C106" s="16"/>
-      <c r="D106" s="15"/>
-      <c r="E106" s="15"/>
+      <c r="D106" s="26"/>
+      <c r="E106" s="27"/>
       <c r="F106" s="14"/>
-      <c r="G106" s="19"/>
+      <c r="G106" s="16"/>
       <c r="H106" s="19"/>
       <c r="I106" s="19"/>
       <c r="J106" s="14">
@@ -4269,10 +4269,10 @@
       <c r="A107" s="28"/>
       <c r="B107" s="16"/>
       <c r="C107" s="16"/>
-      <c r="D107" s="15"/>
-      <c r="E107" s="15"/>
+      <c r="D107" s="26"/>
+      <c r="E107" s="27"/>
       <c r="F107" s="14"/>
-      <c r="G107" s="19"/>
+      <c r="G107" s="16"/>
       <c r="H107" s="19"/>
       <c r="I107" s="19"/>
       <c r="J107" s="14">
@@ -4293,111 +4293,201 @@
       <c r="S107" s="16"/>
     </row>
     <row r="108" spans="1:19" ht="27" customHeight="1">
-      <c r="A108" s="33" t="s">
+      <c r="A108" s="28"/>
+      <c r="B108" s="16"/>
+      <c r="C108" s="16"/>
+      <c r="D108" s="26"/>
+      <c r="E108" s="27"/>
+      <c r="F108" s="14"/>
+      <c r="G108" s="16"/>
+      <c r="H108" s="19"/>
+      <c r="I108" s="19"/>
+      <c r="J108" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K108" s="14"/>
+      <c r="L108" s="16"/>
+      <c r="M108" s="16"/>
+      <c r="N108" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O108" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P108" s="16"/>
+      <c r="Q108" s="13"/>
+      <c r="R108" s="16"/>
+      <c r="S108" s="16"/>
+    </row>
+    <row r="109" spans="1:19" ht="27" customHeight="1">
+      <c r="A109" s="28"/>
+      <c r="B109" s="16"/>
+      <c r="C109" s="16"/>
+      <c r="D109" s="26"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="14"/>
+      <c r="G109" s="16"/>
+      <c r="H109" s="19"/>
+      <c r="I109" s="19"/>
+      <c r="J109" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K109" s="14"/>
+      <c r="L109" s="16"/>
+      <c r="M109" s="16"/>
+      <c r="N109" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O109" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P109" s="16"/>
+      <c r="Q109" s="13"/>
+      <c r="R109" s="16"/>
+      <c r="S109" s="16"/>
+    </row>
+    <row r="110" spans="1:19" ht="27" customHeight="1">
+      <c r="A110" s="28"/>
+      <c r="B110" s="16"/>
+      <c r="C110" s="16"/>
+      <c r="D110" s="26"/>
+      <c r="E110" s="27"/>
+      <c r="F110" s="14"/>
+      <c r="G110" s="16"/>
+      <c r="H110" s="19"/>
+      <c r="I110" s="19"/>
+      <c r="J110" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K110" s="14"/>
+      <c r="L110" s="16"/>
+      <c r="M110" s="16"/>
+      <c r="N110" s="14">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="O110" s="14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="P110" s="16"/>
+      <c r="Q110" s="13"/>
+      <c r="R110" s="16"/>
+      <c r="S110" s="16"/>
+    </row>
+    <row r="111" spans="1:19" ht="27" customHeight="1">
+      <c r="A111" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B108" s="34"/>
-      <c r="C108" s="34"/>
-      <c r="D108" s="35"/>
-      <c r="E108" s="5"/>
-      <c r="F108" s="6"/>
-      <c r="G108" s="6"/>
-      <c r="H108" s="6"/>
-      <c r="I108" s="6"/>
-      <c r="J108" s="7">
+      <c r="B111" s="34"/>
+      <c r="C111" s="34"/>
+      <c r="D111" s="35"/>
+      <c r="E111" s="5"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+      <c r="J111" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="K108" s="7">
-        <f>N108+O108</f>
-        <v>0</v>
-      </c>
-      <c r="L108" s="7">
-        <f>SUM(L5:L107)/2</f>
-        <v>0</v>
-      </c>
-      <c r="M108" s="7">
-        <f>SUM(M5:M107)/2</f>
-        <v>0</v>
-      </c>
-      <c r="N108" s="7">
-        <f>SUM(N5:N107)/2</f>
-        <v>0</v>
-      </c>
-      <c r="O108" s="7">
-        <f>SUM(O5:O107)/2</f>
-        <v>0</v>
-      </c>
-      <c r="P108" s="7">
-        <f>SUM(P5:P107)/2</f>
-        <v>0</v>
-      </c>
-      <c r="Q108" s="7">
-        <f>SUM(Q5:Q107)/2</f>
-        <v>0</v>
-      </c>
-      <c r="R108" s="7">
-        <f>SUM(R5:R107)/2</f>
-        <v>0</v>
-      </c>
-      <c r="S108" s="7">
-        <f>SUM(S5:S107)/2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:19" ht="30" customHeight="1" thickBot="1">
-      <c r="A109" s="36" t="s">
+      <c r="K111" s="7">
+        <f>N111+O111</f>
+        <v>0</v>
+      </c>
+      <c r="L111" s="7">
+        <f>SUM(L5:L110)/2</f>
+        <v>0</v>
+      </c>
+      <c r="M111" s="7">
+        <f>SUM(M5:M110)/2</f>
+        <v>0</v>
+      </c>
+      <c r="N111" s="7">
+        <f>SUM(N5:N110)/2</f>
+        <v>0</v>
+      </c>
+      <c r="O111" s="7">
+        <f>SUM(O5:O110)/2</f>
+        <v>0</v>
+      </c>
+      <c r="P111" s="7">
+        <f>SUM(P5:P110)/2</f>
+        <v>0</v>
+      </c>
+      <c r="Q111" s="7">
+        <f>SUM(Q5:Q110)/2</f>
+        <v>0</v>
+      </c>
+      <c r="R111" s="7">
+        <f>SUM(R5:R110)/2</f>
+        <v>0</v>
+      </c>
+      <c r="S111" s="7">
+        <f>SUM(S5:S110)/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" ht="30" customHeight="1" thickBot="1">
+      <c r="A112" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B109" s="37"/>
-      <c r="C109" s="37"/>
-      <c r="D109" s="37"/>
-      <c r="E109" s="8"/>
-      <c r="F109" s="6"/>
-      <c r="G109" s="6"/>
-      <c r="H109" s="6"/>
-      <c r="I109" s="6"/>
-      <c r="J109" s="30" t="e">
-        <f>(M108+S108)/J108</f>
+      <c r="B112" s="37"/>
+      <c r="C112" s="37"/>
+      <c r="D112" s="37"/>
+      <c r="E112" s="8"/>
+      <c r="F112" s="6"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="6"/>
+      <c r="I112" s="6"/>
+      <c r="J112" s="30" t="e">
+        <f>(M111+S111)/J111</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K109" s="9"/>
-      <c r="L109" s="1"/>
-      <c r="M109" s="1"/>
-      <c r="N109" s="38" t="s">
+      <c r="K112" s="9"/>
+      <c r="L112" s="1"/>
+      <c r="M112" s="1"/>
+      <c r="N112" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="O109" s="39"/>
-      <c r="P109" s="40"/>
-      <c r="Q109" s="9"/>
-      <c r="R109" s="1"/>
-      <c r="S109" s="10"/>
-    </row>
-    <row r="110" spans="1:19" ht="16.2" thickTop="1">
-      <c r="A110" s="31" t="s">
+      <c r="O112" s="39"/>
+      <c r="P112" s="40"/>
+      <c r="Q112" s="9"/>
+      <c r="R112" s="1"/>
+      <c r="S112" s="10"/>
+    </row>
+    <row r="113" spans="1:19" ht="16.2" thickTop="1">
+      <c r="A113" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B110" s="32"/>
-      <c r="C110" s="32"/>
-      <c r="D110" s="32"/>
-      <c r="E110" s="32"/>
-      <c r="F110" s="32"/>
-      <c r="G110" s="32"/>
-      <c r="H110" s="32"/>
-      <c r="I110" s="32"/>
-      <c r="J110" s="32"/>
-      <c r="K110" s="32"/>
-      <c r="L110" s="32"/>
-      <c r="M110" s="32"/>
-      <c r="N110" s="32"/>
-      <c r="O110" s="32"/>
-      <c r="P110" s="32"/>
-      <c r="Q110" s="32"/>
-      <c r="R110" s="32"/>
-      <c r="S110" s="32"/>
-    </row>
-    <row r="113" spans="10:10">
-      <c r="J113" s="11"/>
+      <c r="B113" s="32"/>
+      <c r="C113" s="32"/>
+      <c r="D113" s="32"/>
+      <c r="E113" s="32"/>
+      <c r="F113" s="32"/>
+      <c r="G113" s="32"/>
+      <c r="H113" s="32"/>
+      <c r="I113" s="32"/>
+      <c r="J113" s="32"/>
+      <c r="K113" s="32"/>
+      <c r="L113" s="32"/>
+      <c r="M113" s="32"/>
+      <c r="N113" s="32"/>
+      <c r="O113" s="32"/>
+      <c r="P113" s="32"/>
+      <c r="Q113" s="32"/>
+      <c r="R113" s="32"/>
+      <c r="S113" s="32"/>
+    </row>
+    <row r="116" spans="1:19">
+      <c r="J116" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -4416,10 +4506,10 @@
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="O3:O4"/>
     <mergeCell ref="P3:P4"/>
-    <mergeCell ref="A110:S110"/>
-    <mergeCell ref="A108:D108"/>
-    <mergeCell ref="A109:D109"/>
-    <mergeCell ref="N109:P109"/>
+    <mergeCell ref="A113:S113"/>
+    <mergeCell ref="A111:D111"/>
+    <mergeCell ref="A112:D112"/>
+    <mergeCell ref="N112:P112"/>
     <mergeCell ref="Q3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>